<commit_message>
template and static july
</commit_message>
<xml_diff>
--- a/config/finance/static/template.xlsx
+++ b/config/finance/static/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Financial\config\finance\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E397101-CA0A-44C0-B7CD-FA799A447E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D115E33-6A80-455E-9828-87CC307DF272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRST" sheetId="6" r:id="rId1"/>
@@ -101,11 +101,6 @@
     <t>Depreciation and Amortization</t>
   </si>
   <si>
-    <t>ADVANTAGE ACADEMY 
-FY2022-2023 Statement of 
-Activities as of July 1, 2023</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
@@ -128,10 +123,6 @@
     <t/>
   </si>
   <si>
-    <t>ADVANTAGE ACADEMY
-FY2022-2023 Balance Sheet as of  July 1, 2023</t>
-  </si>
-  <si>
     <t>Statement of Cash Flows</t>
   </si>
   <si>
@@ -223,9 +214,6 @@
   </si>
   <si>
     <t>Cash at End of Period</t>
-  </si>
-  <si>
-    <t>for the period ended of July 1, 2023</t>
   </si>
   <si>
     <t>ADVANTAGE ACADEMY</t>
@@ -423,9 +411,6 @@
     <t xml:space="preserve">            </t>
   </si>
   <si>
-    <t>FY2022-2023 Charter FIRST Forecastas of July 1 2023</t>
-  </si>
-  <si>
     <t>ADVANTAGE ACADAMEY</t>
   </si>
   <si>
@@ -436,6 +421,21 @@
   </si>
   <si>
     <t>As of July</t>
+  </si>
+  <si>
+    <t>FY2022-2023 Charter FIRST Forecastas of July 31, 2023</t>
+  </si>
+  <si>
+    <t>ADVANTAGE ACADEMY 
+FY2022-2023 Statement of 
+Activities as of July 31, 2023</t>
+  </si>
+  <si>
+    <t>ADVANTAGE ACADEMY
+FY2022-2023 Balance Sheet as of  July 31, 2023</t>
+  </si>
+  <si>
+    <t>for the period ended of July 31, 2023</t>
   </si>
 </sst>
 </file>
@@ -4487,7 +4487,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="133.42578125" defaultRowHeight="15"/>
   <cols>
@@ -4503,7 +4503,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21">
       <c r="A1" s="65" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -4512,7 +4512,7 @@
     </row>
     <row r="2" spans="1:5" ht="23.25" customHeight="1">
       <c r="A2" s="67" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B2" s="67"/>
       <c r="C2" s="67"/>
@@ -4521,67 +4521,67 @@
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="E3" s="68" t="s">
         <v>63</v>
-      </c>
-      <c r="C3" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
       <c r="A4" s="70" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4" s="71">
         <v>-1323478</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="73"/>
       <c r="E4" s="74"/>
     </row>
     <row r="5" spans="1:5" ht="45">
       <c r="A5" s="75" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="75" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="76"/>
       <c r="E5" s="77" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="70" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" s="76"/>
       <c r="E6" s="80" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="70" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B7" s="81">
         <v>190</v>
@@ -4591,12 +4591,12 @@
       </c>
       <c r="D7" s="76"/>
       <c r="E7" s="80" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
       <c r="A8" s="82" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="83">
         <v>4.6100000000000003</v>
@@ -4606,12 +4606,12 @@
       </c>
       <c r="D8" s="76"/>
       <c r="E8" s="80" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
       <c r="A9" s="82" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="71">
         <v>-802645</v>
@@ -4621,27 +4621,27 @@
       </c>
       <c r="D9" s="85"/>
       <c r="E9" s="80" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="82" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" s="84">
         <v>10</v>
       </c>
       <c r="D10" s="76"/>
       <c r="E10" s="80" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="82" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11" s="83">
         <v>0.64</v>
@@ -4651,27 +4651,27 @@
       </c>
       <c r="D11" s="76"/>
       <c r="E11" s="80" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="82" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" s="86" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C12" s="84">
         <v>10</v>
       </c>
       <c r="D12" s="76"/>
       <c r="E12" s="80" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="82" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B13" s="87">
         <v>0.68</v>
@@ -4681,132 +4681,132 @@
       </c>
       <c r="D13" s="76"/>
       <c r="E13" s="80" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="A14" s="88" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B14" s="89" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C14" s="78">
         <v>10</v>
       </c>
       <c r="D14" s="76"/>
       <c r="E14" s="90" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
       <c r="A15" s="91" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" s="78">
         <v>10</v>
       </c>
       <c r="D15" s="76"/>
       <c r="E15" s="80" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="82" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C16" s="84">
         <v>5</v>
       </c>
       <c r="D16" s="76"/>
       <c r="E16" s="80" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="82" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B17" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D17" s="76"/>
       <c r="E17" s="80" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="82" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B18" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18" s="76"/>
       <c r="E18" s="80" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="82" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B19" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C19" s="84">
         <v>10</v>
       </c>
       <c r="D19" s="76"/>
       <c r="E19" s="80" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="34.15" customHeight="1">
       <c r="A20" s="82" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B20" s="78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="84">
         <v>5</v>
       </c>
       <c r="D20" s="76"/>
       <c r="E20" s="80" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30">
       <c r="A21" s="91" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D21" s="76"/>
       <c r="E21" s="80" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="34.15" customHeight="1">
       <c r="A22" s="92" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="109">
         <v>100</v>
@@ -4814,15 +4814,15 @@
       <c r="C22" s="110"/>
       <c r="D22" s="111"/>
       <c r="E22" s="113" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="34.15" customHeight="1">
       <c r="A23" s="93" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B23" s="115" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C23" s="116"/>
       <c r="D23" s="112"/>
@@ -4843,7 +4843,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="96" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B26" s="94"/>
       <c r="C26" s="94"/>
@@ -4902,7 +4902,7 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:X1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4926,7 +4926,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="108" customHeight="1">
       <c r="B1" s="117" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="C1" s="117"/>
       <c r="D1" s="117"/>
@@ -7581,7 +7581,7 @@
   </sheetPr>
   <dimension ref="A1:Z119"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -7608,7 +7608,7 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
       <c r="D1" s="19" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
@@ -7634,7 +7634,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="24"/>
       <c r="F2" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -7667,10 +7667,10 @@
       </c>
       <c r="S2" s="23"/>
       <c r="T2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="77.25" customHeight="1" collapsed="1">
@@ -7678,7 +7678,7 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="F3" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>1</v>
@@ -7718,20 +7718,20 @@
       </c>
       <c r="S3" s="26"/>
       <c r="T3" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U3" s="27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15">
       <c r="D4" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="28"/>
       <c r="T4" s="29"/>
       <c r="U4" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15">
@@ -10328,7 +10328,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="20.25">
       <c r="A1" s="40" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -10349,7 +10349,7 @@
     </row>
     <row r="2" spans="1:18" ht="20.25">
       <c r="A2" s="40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -10370,7 +10370,7 @@
     </row>
     <row r="3" spans="1:18" ht="20.25">
       <c r="A3" s="40" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -10405,7 +10405,7 @@
       <c r="O4" s="43"/>
       <c r="P4" s="58"/>
       <c r="Q4" s="42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R4" s="44"/>
     </row>
@@ -10447,12 +10447,12 @@
         <v>12</v>
       </c>
       <c r="Q5" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15">
       <c r="A6" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -10473,7 +10473,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="46">
         <v>-1375582</v>
@@ -10548,10 +10548,10 @@
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="29">
         <v>589378</v>
@@ -10578,7 +10578,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="29">
         <v>20990</v>
@@ -10608,7 +10608,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
@@ -10623,12 +10623,12 @@
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
       <c r="Q12" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="B13" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="29">
         <v>181842</v>
@@ -10658,22 +10658,22 @@
     </row>
     <row r="14" spans="1:18">
       <c r="B14" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F14" s="29">
         <v>1080</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I14" s="29"/>
       <c r="J14" s="60"/>
@@ -10688,22 +10688,22 @@
     </row>
     <row r="15" spans="1:18" hidden="1" outlineLevel="1">
       <c r="B15" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="60"/>
@@ -10716,22 +10716,22 @@
     </row>
     <row r="16" spans="1:18" hidden="1" outlineLevel="1">
       <c r="B16" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="60"/>
@@ -10744,22 +10744,22 @@
     </row>
     <row r="17" spans="1:17" hidden="1" outlineLevel="1">
       <c r="B17" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="60"/>
@@ -10787,7 +10787,7 @@
     </row>
     <row r="19" spans="1:17" ht="15">
       <c r="A19" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="51">
         <v>-1068584</v>
@@ -10847,7 +10847,7 @@
     </row>
     <row r="22" spans="1:17" ht="15">
       <c r="A22" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -10868,25 +10868,25 @@
     <row r="23" spans="1:17" ht="15">
       <c r="A23" s="24"/>
       <c r="B23" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="53">
         <v>1510</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F23" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G23" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H23" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I23" s="46"/>
       <c r="J23" s="47"/>
@@ -10895,30 +10895,30 @@
       <c r="M23" s="47"/>
       <c r="O23" s="47"/>
       <c r="Q23" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="B24" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="53">
         <v>1520</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E24" s="29">
         <v>-132300</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I24" s="29"/>
       <c r="J24" s="60"/>
@@ -10933,25 +10933,25 @@
     </row>
     <row r="25" spans="1:17">
       <c r="B25" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="53">
         <v>1538</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E25" s="29">
         <v>-139</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G25" s="29">
         <v>-21374</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="60"/>
@@ -10966,25 +10966,25 @@
     </row>
     <row r="26" spans="1:17">
       <c r="B26" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" s="53">
         <v>1539</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I26" s="29"/>
       <c r="J26" s="60"/>
@@ -10994,12 +10994,12 @@
       <c r="N26" s="60"/>
       <c r="O26" s="60"/>
       <c r="Q26" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="B27" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" s="53">
         <v>1531</v>
@@ -11008,16 +11008,16 @@
         <v>-231</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I27" s="29"/>
       <c r="J27" s="60"/>
@@ -11032,22 +11032,22 @@
     </row>
     <row r="28" spans="1:17">
       <c r="B28" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I28" s="29"/>
       <c r="J28" s="60"/>
@@ -11057,7 +11057,7 @@
       <c r="N28" s="60"/>
       <c r="O28" s="60"/>
       <c r="Q28" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -11077,7 +11077,7 @@
     </row>
     <row r="30" spans="1:17" ht="15">
       <c r="A30" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
@@ -11135,7 +11135,7 @@
     </row>
     <row r="33" spans="1:22" ht="15">
       <c r="A33" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -11155,7 +11155,7 @@
     </row>
     <row r="34" spans="1:22">
       <c r="B34" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34" s="57"/>
       <c r="E34" s="57"/>
@@ -11173,7 +11173,7 @@
     </row>
     <row r="35" spans="1:22">
       <c r="B35" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
@@ -11191,7 +11191,7 @@
     </row>
     <row r="36" spans="1:22">
       <c r="B36" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D36" s="57"/>
       <c r="E36" s="57"/>
@@ -11209,46 +11209,46 @@
     </row>
     <row r="37" spans="1:22">
       <c r="D37" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E37" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F37" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G37" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H37" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I37" s="49"/>
       <c r="J37" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K37" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L37" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M37" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N37" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O37" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q37" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="15">
       <c r="A38" s="24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -11268,46 +11268,46 @@
     </row>
     <row r="39" spans="1:22">
       <c r="D39" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G39" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H39" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I39" s="49"/>
       <c r="J39" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K39" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L39" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M39" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N39" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O39" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q39" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="15">
       <c r="A40" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D40" s="51">
         <v>-1068815</v>
@@ -11352,7 +11352,7 @@
     </row>
     <row r="42" spans="1:22" ht="15">
       <c r="A42" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D42" s="51">
         <v>7264371</v>
@@ -11382,46 +11382,46 @@
     </row>
     <row r="43" spans="1:22">
       <c r="D43" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E43" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F43" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G43" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H43" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I43" s="49"/>
       <c r="J43" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K43" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L43" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M43" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O43" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q43" s="49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15.75" thickBot="1">
       <c r="A44" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D44" s="54">
         <v>6195556</v>

</xml_diff>

<commit_message>
pl dna and total fix
</commit_message>
<xml_diff>
--- a/config/finance/static/template.xlsx
+++ b/config/finance/static/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Financial\config\finance\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D115E33-6A80-455E-9828-87CC307DF272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0218A78E-7FFB-4D29-91F9-5171408B5DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRST" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">BS!$D$1:$U$92</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Cash Flow Statement'!$A$1:$Q$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">PL!$B$1:$V$146</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">PL!$B$1:$V$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4487,7 +4487,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="133.42578125" defaultRowHeight="15"/>
   <cols>
@@ -7581,7 +7581,7 @@
   </sheetPr>
   <dimension ref="A1:Z119"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -11472,6 +11472,6 @@
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="36" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel pl hide rows
</commit_message>
<xml_diff>
--- a/config/finance/static/template.xlsx
+++ b/config/finance/static/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Financial\config\finance\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BC02A5-9506-4D38-AD87-78948919BFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1861A11-8E1B-447B-BA3C-9055C33763ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,22 +394,22 @@
     <t>10.3% / 10.2%</t>
   </si>
   <si>
-    <t>As of July</t>
-  </si>
-  <si>
-    <t>FY2022-2023 Charter FIRST Forecastas of July 31, 2023</t>
+    <t>FY2022-2023 Charter FIRST Forecastas of August 31, 2023</t>
   </si>
   <si>
     <t>ADVANTAGE ACADEMY 
 FY2022-2023 Statement of 
-Activities as of July 31, 2023</t>
+Activities as of August 31, 2023</t>
   </si>
   <si>
     <t>ADVANTAGE ACADEMY
-FY2022-2023 Balance Sheet as of  July 31, 2023</t>
+FY2022-2023 Balance Sheet as of August 31, 2023</t>
   </si>
   <si>
-    <t>for the period ended of July 31, 2023</t>
+    <t>As of August</t>
+  </si>
+  <si>
+    <t>for the period ended o fAugust 31, 2023</t>
   </si>
 </sst>
 </file>
@@ -4456,9 +4456,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="133.42578125" defaultRowHeight="15"/>
   <cols>
@@ -4483,7 +4481,7 @@
     </row>
     <row r="2" spans="1:5" ht="23.25" customHeight="1">
       <c r="A2" s="62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="62"/>
       <c r="C2" s="62"/>
@@ -4897,7 +4895,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="108" customHeight="1">
       <c r="B1" s="112" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="112"/>
       <c r="D1" s="112"/>
@@ -5636,7 +5634,7 @@
       <c r="U34" s="14"/>
       <c r="V34" s="8"/>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" hidden="1" outlineLevel="1">
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -5699,7 +5697,7 @@
       <c r="U37" s="6"/>
       <c r="V37" s="11"/>
     </row>
-    <row r="38" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="38" spans="1:22" collapsed="1">
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -5720,7 +5718,7 @@
       <c r="U38" s="6"/>
       <c r="V38" s="11"/>
     </row>
-    <row r="39" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="39" spans="1:22">
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -5741,7 +5739,7 @@
       <c r="U39" s="6"/>
       <c r="V39" s="11"/>
     </row>
-    <row r="40" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="40" spans="1:22">
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -5762,7 +5760,7 @@
       <c r="U40" s="6"/>
       <c r="V40" s="11"/>
     </row>
-    <row r="41" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="41" spans="1:22">
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -5783,7 +5781,7 @@
       <c r="U41" s="6"/>
       <c r="V41" s="11"/>
     </row>
-    <row r="42" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="42" spans="1:22">
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -5804,7 +5802,7 @@
       <c r="U42" s="6"/>
       <c r="V42" s="11"/>
     </row>
-    <row r="43" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="43" spans="1:22">
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -5825,7 +5823,7 @@
       <c r="U43" s="6"/>
       <c r="V43" s="11"/>
     </row>
-    <row r="44" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="44" spans="1:22">
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -5846,7 +5844,7 @@
       <c r="U44" s="6"/>
       <c r="V44" s="11"/>
     </row>
-    <row r="45" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="45" spans="1:22">
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -5867,7 +5865,7 @@
       <c r="U45" s="6"/>
       <c r="V45" s="11"/>
     </row>
-    <row r="46" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:22">
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -5888,7 +5886,7 @@
       <c r="U46" s="6"/>
       <c r="V46" s="11"/>
     </row>
-    <row r="47" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="47" spans="1:22">
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -5909,7 +5907,7 @@
       <c r="U47" s="6"/>
       <c r="V47" s="11"/>
     </row>
-    <row r="48" spans="1:22" hidden="1" outlineLevel="1">
+    <row r="48" spans="1:22">
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -5930,7 +5928,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="11"/>
     </row>
-    <row r="49" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="49" spans="2:22">
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
@@ -5951,7 +5949,7 @@
       <c r="U49" s="6"/>
       <c r="V49" s="11"/>
     </row>
-    <row r="50" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="50" spans="2:22">
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -5972,7 +5970,7 @@
       <c r="U50" s="6"/>
       <c r="V50" s="11"/>
     </row>
-    <row r="51" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="51" spans="2:22">
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -5993,7 +5991,7 @@
       <c r="U51" s="6"/>
       <c r="V51" s="11"/>
     </row>
-    <row r="52" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="52" spans="2:22">
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
@@ -6014,7 +6012,7 @@
       <c r="U52" s="6"/>
       <c r="V52" s="11"/>
     </row>
-    <row r="53" spans="2:22" collapsed="1">
+    <row r="53" spans="2:22">
       <c r="B53" s="4"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -6064,7 +6062,7 @@
     <row r="56" spans="2:22">
       <c r="V56" s="11"/>
     </row>
-    <row r="57" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="57" spans="2:22">
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -6211,7 +6209,7 @@
       <c r="U63" s="6"/>
       <c r="V63" s="11"/>
     </row>
-    <row r="64" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="64" spans="2:22">
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -6232,7 +6230,7 @@
       <c r="U64" s="6"/>
       <c r="V64" s="11"/>
     </row>
-    <row r="65" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="65" spans="2:22">
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
@@ -6253,7 +6251,7 @@
       <c r="U65" s="6"/>
       <c r="V65" s="11"/>
     </row>
-    <row r="66" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="66" spans="2:22">
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -6274,7 +6272,7 @@
       <c r="U66" s="6"/>
       <c r="V66" s="11"/>
     </row>
-    <row r="67" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="67" spans="2:22">
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -6295,7 +6293,7 @@
       <c r="U67" s="6"/>
       <c r="V67" s="11"/>
     </row>
-    <row r="68" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="68" spans="2:22">
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
@@ -6316,7 +6314,7 @@
       <c r="U68" s="6"/>
       <c r="V68" s="11"/>
     </row>
-    <row r="69" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="69" spans="2:22">
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -6337,7 +6335,7 @@
       <c r="U69" s="6"/>
       <c r="V69" s="11"/>
     </row>
-    <row r="70" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="70" spans="2:22">
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -6358,7 +6356,7 @@
       <c r="U70" s="6"/>
       <c r="V70" s="11"/>
     </row>
-    <row r="71" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="71" spans="2:22">
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
@@ -6379,7 +6377,7 @@
       <c r="U71" s="6"/>
       <c r="V71" s="11"/>
     </row>
-    <row r="72" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="72" spans="2:22">
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -6400,7 +6398,7 @@
       <c r="U72" s="6"/>
       <c r="V72" s="11"/>
     </row>
-    <row r="73" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="73" spans="2:22">
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -6421,7 +6419,7 @@
       <c r="U73" s="6"/>
       <c r="V73" s="11"/>
     </row>
-    <row r="74" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="74" spans="2:22">
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
@@ -6442,7 +6440,7 @@
       <c r="U74" s="6"/>
       <c r="V74" s="11"/>
     </row>
-    <row r="75" spans="2:22" collapsed="1">
+    <row r="75" spans="2:22">
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -6463,7 +6461,7 @@
       <c r="U75" s="6"/>
       <c r="V75" s="11"/>
     </row>
-    <row r="76" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="76" spans="2:22">
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
@@ -6484,7 +6482,7 @@
       <c r="U76" s="6"/>
       <c r="V76" s="11"/>
     </row>
-    <row r="77" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="77" spans="2:22">
       <c r="B77" s="99"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
@@ -6506,7 +6504,7 @@
       <c r="U77" s="6"/>
       <c r="V77" s="11"/>
     </row>
-    <row r="78" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="78" spans="2:22">
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -6527,7 +6525,7 @@
       <c r="U78" s="6"/>
       <c r="V78" s="11"/>
     </row>
-    <row r="79" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="79" spans="2:22">
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
@@ -6548,7 +6546,7 @@
       <c r="U79" s="6"/>
       <c r="V79" s="11"/>
     </row>
-    <row r="80" spans="2:22" hidden="1" outlineLevel="1">
+    <row r="80" spans="2:22">
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -6569,7 +6567,7 @@
       <c r="U80" s="6"/>
       <c r="V80" s="11"/>
     </row>
-    <row r="81" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="81" spans="3:22">
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
@@ -6590,7 +6588,7 @@
       <c r="U81" s="6"/>
       <c r="V81" s="11"/>
     </row>
-    <row r="82" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="82" spans="3:22">
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
@@ -6611,7 +6609,7 @@
       <c r="U82" s="6"/>
       <c r="V82" s="11"/>
     </row>
-    <row r="83" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="83" spans="3:22">
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
@@ -6632,7 +6630,7 @@
       <c r="U83" s="6"/>
       <c r="V83" s="11"/>
     </row>
-    <row r="84" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="84" spans="3:22">
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
@@ -6653,7 +6651,7 @@
       <c r="U84" s="6"/>
       <c r="V84" s="11"/>
     </row>
-    <row r="85" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="85" spans="3:22">
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="F85" s="6"/>
@@ -6674,7 +6672,7 @@
       <c r="U85" s="6"/>
       <c r="V85" s="11"/>
     </row>
-    <row r="86" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="86" spans="3:22">
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
       <c r="F86" s="6"/>
@@ -6695,7 +6693,7 @@
       <c r="U86" s="6"/>
       <c r="V86" s="11"/>
     </row>
-    <row r="87" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="87" spans="3:22">
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
@@ -6716,7 +6714,7 @@
       <c r="U87" s="6"/>
       <c r="V87" s="11"/>
     </row>
-    <row r="88" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="88" spans="3:22">
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
@@ -6737,7 +6735,7 @@
       <c r="U88" s="6"/>
       <c r="V88" s="11"/>
     </row>
-    <row r="89" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="89" spans="3:22">
       <c r="C89" s="4"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
@@ -6759,7 +6757,7 @@
       <c r="U89" s="6"/>
       <c r="V89" s="11"/>
     </row>
-    <row r="90" spans="3:22" collapsed="1">
+    <row r="90" spans="3:22">
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
@@ -6780,7 +6778,7 @@
       <c r="U90" s="6"/>
       <c r="V90" s="11"/>
     </row>
-    <row r="91" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="91" spans="3:22">
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="F91" s="6"/>
@@ -6801,7 +6799,7 @@
       <c r="U91" s="6"/>
       <c r="V91" s="11"/>
     </row>
-    <row r="92" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="92" spans="3:22">
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
@@ -6822,7 +6820,7 @@
       <c r="U92" s="6"/>
       <c r="V92" s="11"/>
     </row>
-    <row r="93" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="93" spans="3:22">
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
       <c r="F93" s="6"/>
@@ -6843,7 +6841,7 @@
       <c r="U93" s="6"/>
       <c r="V93" s="11"/>
     </row>
-    <row r="94" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="94" spans="3:22">
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
       <c r="F94" s="6"/>
@@ -6864,7 +6862,7 @@
       <c r="U94" s="6"/>
       <c r="V94" s="11"/>
     </row>
-    <row r="95" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="95" spans="3:22">
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
       <c r="F95" s="6"/>
@@ -6885,7 +6883,7 @@
       <c r="U95" s="6"/>
       <c r="V95" s="11"/>
     </row>
-    <row r="96" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="96" spans="3:22">
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
@@ -6906,7 +6904,7 @@
       <c r="U96" s="6"/>
       <c r="V96" s="11"/>
     </row>
-    <row r="97" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="97" spans="3:22">
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="F97" s="6"/>
@@ -6927,7 +6925,7 @@
       <c r="U97" s="6"/>
       <c r="V97" s="11"/>
     </row>
-    <row r="98" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="98" spans="3:22">
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
@@ -6948,7 +6946,7 @@
       <c r="U98" s="6"/>
       <c r="V98" s="11"/>
     </row>
-    <row r="99" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="99" spans="3:22">
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
@@ -6969,7 +6967,7 @@
       <c r="U99" s="6"/>
       <c r="V99" s="11"/>
     </row>
-    <row r="100" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="100" spans="3:22">
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
       <c r="F100" s="6"/>
@@ -6990,7 +6988,7 @@
       <c r="U100" s="6"/>
       <c r="V100" s="11"/>
     </row>
-    <row r="101" spans="3:22" collapsed="1">
+    <row r="101" spans="3:22">
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
@@ -7011,7 +7009,7 @@
       <c r="U101" s="6"/>
       <c r="V101" s="11"/>
     </row>
-    <row r="102" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="102" spans="3:22">
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -7032,7 +7030,7 @@
       <c r="U102" s="6"/>
       <c r="V102" s="11"/>
     </row>
-    <row r="103" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="103" spans="3:22">
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
       <c r="F103" s="6"/>
@@ -7053,7 +7051,7 @@
       <c r="U103" s="6"/>
       <c r="V103" s="11"/>
     </row>
-    <row r="104" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="104" spans="3:22">
       <c r="C104" s="4"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
@@ -7075,7 +7073,7 @@
       <c r="U104" s="6"/>
       <c r="V104" s="103"/>
     </row>
-    <row r="105" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="105" spans="3:22">
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
       <c r="F105" s="6"/>
@@ -7096,7 +7094,7 @@
       <c r="U105" s="6"/>
       <c r="V105" s="11"/>
     </row>
-    <row r="106" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="106" spans="3:22">
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
       <c r="F106" s="6"/>
@@ -7117,7 +7115,7 @@
       <c r="U106" s="6"/>
       <c r="V106" s="11"/>
     </row>
-    <row r="107" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="107" spans="3:22">
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
       <c r="F107" s="6"/>
@@ -7138,7 +7136,7 @@
       <c r="U107" s="6"/>
       <c r="V107" s="11"/>
     </row>
-    <row r="108" spans="3:22" collapsed="1">
+    <row r="108" spans="3:22">
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
       <c r="F108" s="6"/>
@@ -7159,7 +7157,7 @@
       <c r="U108" s="6"/>
       <c r="V108" s="11"/>
     </row>
-    <row r="109" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="109" spans="3:22">
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
       <c r="F109" s="6"/>
@@ -7180,7 +7178,7 @@
       <c r="U109" s="6"/>
       <c r="V109" s="11"/>
     </row>
-    <row r="110" spans="3:22" hidden="1" outlineLevel="1">
+    <row r="110" spans="3:22">
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
@@ -7201,7 +7199,7 @@
       <c r="U110" s="6"/>
       <c r="V110" s="11"/>
     </row>
-    <row r="111" spans="3:22" collapsed="1">
+    <row r="111" spans="3:22">
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
       <c r="F111" s="6"/>
@@ -7579,7 +7577,7 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
       <c r="D1" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
@@ -7692,7 +7690,7 @@
         <v>22</v>
       </c>
       <c r="U3" s="27" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15">
@@ -10279,9 +10277,7 @@
   </sheetPr>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>

</xml_diff>

<commit_message>
first and pl excel
</commit_message>
<xml_diff>
--- a/config/finance/static/template.xlsx
+++ b/config/finance/static/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Financial\config\finance\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CC4B77-45A3-432C-8061-7A911EA2B230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88BAD65-06AB-4514-AE0A-E06F316981D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -768,7 +768,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -974,9 +974,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1365,9 +1362,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="133.42578125" defaultRowHeight="15"/>
   <cols>
@@ -1650,10 +1645,10 @@
       <c r="A22" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="99"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="103" t="s">
+      <c r="B22" s="96"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="100" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1661,12 +1656,12 @@
       <c r="A23" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="105" t="s">
+      <c r="B23" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="106"/>
-      <c r="D23" s="102"/>
-      <c r="E23" s="104"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="101"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="85"/>
@@ -1738,10 +1733,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X128"/>
+  <dimension ref="A1:X150"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -1765,31 +1760,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="108" customHeight="1">
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="104" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="107"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
     </row>
     <row r="3" spans="1:24" ht="55.5" customHeight="1">
       <c r="D3" s="3" t="s">
@@ -3942,7 +3937,7 @@
       <c r="S104" s="6"/>
       <c r="T104" s="6"/>
       <c r="U104" s="6"/>
-      <c r="V104" s="97"/>
+      <c r="V104" s="11"/>
     </row>
     <row r="105" spans="3:22">
       <c r="D105" s="6"/>
@@ -4092,70 +4087,70 @@
       <c r="V111" s="11"/>
     </row>
     <row r="112" spans="3:22">
-      <c r="D112" s="98"/>
-      <c r="E112" s="98"/>
-      <c r="F112" s="98"/>
-      <c r="G112" s="98"/>
-      <c r="H112" s="98"/>
-      <c r="I112" s="98"/>
-      <c r="J112" s="98"/>
-      <c r="K112" s="98"/>
-      <c r="L112" s="98"/>
-      <c r="M112" s="98"/>
-      <c r="N112" s="98"/>
-      <c r="O112" s="98"/>
-      <c r="P112" s="98"/>
-      <c r="Q112" s="98"/>
-      <c r="R112" s="98"/>
-      <c r="S112" s="98"/>
-      <c r="T112" s="98"/>
-      <c r="U112" s="98"/>
-      <c r="V112" s="96"/>
+      <c r="D112" s="95"/>
+      <c r="E112" s="95"/>
+      <c r="F112" s="95"/>
+      <c r="G112" s="95"/>
+      <c r="H112" s="95"/>
+      <c r="I112" s="95"/>
+      <c r="J112" s="95"/>
+      <c r="K112" s="95"/>
+      <c r="L112" s="95"/>
+      <c r="M112" s="95"/>
+      <c r="N112" s="95"/>
+      <c r="O112" s="95"/>
+      <c r="P112" s="95"/>
+      <c r="Q112" s="95"/>
+      <c r="R112" s="95"/>
+      <c r="S112" s="95"/>
+      <c r="T112" s="95"/>
+      <c r="U112" s="95"/>
+      <c r="V112" s="11"/>
     </row>
     <row r="113" spans="1:22">
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
-      <c r="D113" s="98"/>
-      <c r="E113" s="98"/>
-      <c r="F113" s="98"/>
-      <c r="G113" s="98"/>
-      <c r="H113" s="98"/>
-      <c r="I113" s="98"/>
-      <c r="J113" s="98"/>
-      <c r="K113" s="98"/>
-      <c r="L113" s="98"/>
-      <c r="M113" s="98"/>
-      <c r="N113" s="98"/>
-      <c r="O113" s="98"/>
-      <c r="P113" s="98"/>
-      <c r="Q113" s="98"/>
-      <c r="R113" s="98"/>
-      <c r="S113" s="98"/>
-      <c r="T113" s="98"/>
-      <c r="U113" s="98"/>
-      <c r="V113" s="96"/>
+      <c r="D113" s="95"/>
+      <c r="E113" s="95"/>
+      <c r="F113" s="95"/>
+      <c r="G113" s="95"/>
+      <c r="H113" s="95"/>
+      <c r="I113" s="95"/>
+      <c r="J113" s="95"/>
+      <c r="K113" s="95"/>
+      <c r="L113" s="95"/>
+      <c r="M113" s="95"/>
+      <c r="N113" s="95"/>
+      <c r="O113" s="95"/>
+      <c r="P113" s="95"/>
+      <c r="Q113" s="95"/>
+      <c r="R113" s="95"/>
+      <c r="S113" s="95"/>
+      <c r="T113" s="95"/>
+      <c r="U113" s="95"/>
+      <c r="V113" s="11"/>
     </row>
     <row r="114" spans="1:22">
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
-      <c r="D114" s="98"/>
-      <c r="E114" s="98"/>
-      <c r="F114" s="98"/>
-      <c r="G114" s="98"/>
-      <c r="H114" s="98"/>
-      <c r="I114" s="98"/>
-      <c r="J114" s="98"/>
-      <c r="K114" s="98"/>
-      <c r="L114" s="98"/>
-      <c r="M114" s="98"/>
-      <c r="N114" s="98"/>
-      <c r="O114" s="98"/>
-      <c r="P114" s="98"/>
-      <c r="Q114" s="98"/>
-      <c r="R114" s="98"/>
-      <c r="S114" s="98"/>
-      <c r="T114" s="98"/>
-      <c r="U114" s="98"/>
+      <c r="D114" s="95"/>
+      <c r="E114" s="95"/>
+      <c r="F114" s="95"/>
+      <c r="G114" s="95"/>
+      <c r="H114" s="95"/>
+      <c r="I114" s="95"/>
+      <c r="J114" s="95"/>
+      <c r="K114" s="95"/>
+      <c r="L114" s="95"/>
+      <c r="M114" s="95"/>
+      <c r="N114" s="95"/>
+      <c r="O114" s="95"/>
+      <c r="P114" s="95"/>
+      <c r="Q114" s="95"/>
+      <c r="R114" s="95"/>
+      <c r="S114" s="95"/>
+      <c r="T114" s="95"/>
+      <c r="U114" s="95"/>
       <c r="V114" s="11"/>
     </row>
     <row r="115" spans="1:22">
@@ -4180,7 +4175,7 @@
       <c r="S115" s="12"/>
       <c r="T115" s="12"/>
       <c r="U115" s="12"/>
-      <c r="V115" s="97"/>
+      <c r="V115" s="11"/>
     </row>
     <row r="116" spans="1:22">
       <c r="D116" s="6"/>
@@ -4306,7 +4301,7 @@
       <c r="S121" s="6"/>
       <c r="T121" s="6"/>
       <c r="U121" s="6"/>
-      <c r="V121" s="94"/>
+      <c r="V121" s="11"/>
     </row>
     <row r="122" spans="1:22">
       <c r="A122" s="4"/>
@@ -4330,7 +4325,7 @@
       <c r="S122" s="12"/>
       <c r="T122" s="12"/>
       <c r="U122" s="12"/>
-      <c r="V122" s="95"/>
+      <c r="V122" s="11"/>
     </row>
     <row r="123" spans="1:22">
       <c r="D123" s="6"/>
@@ -4351,7 +4346,7 @@
       <c r="S123" s="6"/>
       <c r="T123" s="6"/>
       <c r="U123" s="6"/>
-      <c r="V123" s="94"/>
+      <c r="V123" s="11"/>
     </row>
     <row r="124" spans="1:22">
       <c r="D124" s="6"/>
@@ -4372,7 +4367,7 @@
       <c r="S124" s="6"/>
       <c r="T124" s="6"/>
       <c r="U124" s="6"/>
-      <c r="V124" s="94"/>
+      <c r="V124" s="11"/>
     </row>
     <row r="125" spans="1:22">
       <c r="B125" s="4"/>
@@ -4395,13 +4390,84 @@
       <c r="S125" s="12"/>
       <c r="T125" s="12"/>
       <c r="U125" s="4"/>
-      <c r="V125" s="95"/>
+      <c r="V125" s="11"/>
+    </row>
+    <row r="126" spans="1:22">
+      <c r="V126" s="11"/>
     </row>
     <row r="127" spans="1:22">
       <c r="B127" s="4"/>
+      <c r="V127" s="11"/>
     </row>
     <row r="128" spans="1:22">
       <c r="B128" s="4"/>
+      <c r="V128" s="11"/>
+    </row>
+    <row r="129" spans="22:22">
+      <c r="V129" s="11"/>
+    </row>
+    <row r="130" spans="22:22">
+      <c r="V130" s="11"/>
+    </row>
+    <row r="131" spans="22:22">
+      <c r="V131" s="11"/>
+    </row>
+    <row r="132" spans="22:22">
+      <c r="V132" s="11"/>
+    </row>
+    <row r="133" spans="22:22">
+      <c r="V133" s="11"/>
+    </row>
+    <row r="134" spans="22:22">
+      <c r="V134" s="11"/>
+    </row>
+    <row r="135" spans="22:22">
+      <c r="V135" s="11"/>
+    </row>
+    <row r="136" spans="22:22">
+      <c r="V136" s="11"/>
+    </row>
+    <row r="137" spans="22:22">
+      <c r="V137" s="11"/>
+    </row>
+    <row r="138" spans="22:22">
+      <c r="V138" s="11"/>
+    </row>
+    <row r="139" spans="22:22">
+      <c r="V139" s="11"/>
+    </row>
+    <row r="140" spans="22:22">
+      <c r="V140" s="11"/>
+    </row>
+    <row r="141" spans="22:22">
+      <c r="V141" s="11"/>
+    </row>
+    <row r="142" spans="22:22">
+      <c r="V142" s="11"/>
+    </row>
+    <row r="143" spans="22:22">
+      <c r="V143" s="11"/>
+    </row>
+    <row r="144" spans="22:22">
+      <c r="V144" s="11"/>
+    </row>
+    <row r="145" spans="22:22">
+      <c r="V145" s="11"/>
+    </row>
+    <row r="146" spans="22:22">
+      <c r="V146" s="11"/>
+    </row>
+    <row r="147" spans="22:22">
+      <c r="V147" s="11"/>
+    </row>
+    <row r="148" spans="22:22">
+      <c r="V148" s="11"/>
+    </row>
+    <row r="149" spans="22:22">
+      <c r="V149" s="11"/>
+    </row>
+    <row r="150" spans="22:22">
+      <c r="V150" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
excel and village tech budget
</commit_message>
<xml_diff>
--- a/config/finance/static/template.xlsx
+++ b/config/finance/static/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Financial\config\finance\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626A2BF8-B9FC-4A01-AE27-A71F62CA4599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02ADC9C-5DCD-44CC-9624-5B7C204304D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRST" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">BS!$D$1:$U$128</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Cash Flow Statement'!$A$1:$Q$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">FIRST!$A$1:$E$23</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">PL!$B$1:$V$170</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">PL!$B$1:$V$114</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1339,7 +1339,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="133.42578125" defaultRowHeight="15"/>
   <cols>
@@ -1712,8 +1712,8 @@
   </sheetPr>
   <dimension ref="A1:X150"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -4437,7 +4437,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0"/>
-  <pageSetup scale="28" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="41" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
logo and excel template
</commit_message>
<xml_diff>
--- a/config/finance/static/template.xlsx
+++ b/config/finance/static/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Financial\config\finance\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559DBE46-FECC-4E62-8F01-774D3398DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81EAFD1-C175-44AC-BD53-DD82B208A81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,9 +19,9 @@
     <sheet name="Cash Flow Statement" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">BS!$D$1:$U$128</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">BS!$D$1:$U$65</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Cash Flow Statement'!$A$1:$Q$38</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">FIRST!$A$1:$E$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">FIRST!$A$1:$E$25</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">PL!$B$1:$V$109</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -7042,7 +7042,7 @@
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0"/>
-  <pageSetup scale="38" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="40" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>